<commit_message>
Separate all disease code lists
Separate all disease code lists by SNOMED and read codes (except for Spirometry, as haven't finalised codelist)
</commit_message>
<xml_diff>
--- a/codelists/AECOPD_LRTI.xlsx
+++ b/codelists/AECOPD_LRTI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Group_work\NACAP\2023\Primary care\codelists_received_from_jenni\Finalised_codelists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/hk1923_ic_ac_uk/Documents/Documents/GitHub/primary_care2022/codelists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CA5C74F-163B-4EF6-85FD-9C782A95D2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{7CA5C74F-163B-4EF6-85FD-9C782A95D2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68234438-DE53-4450-BE58-37A85461042E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7845" yWindow="1200" windowWidth="20235" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -1997,12 +1997,13 @@
   <dimension ref="A1:I178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="80.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>